<commit_message>
minor fixes to clear warnings
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CEQextension.xlsx
+++ b/output/StructureDefinition-CEQextension.xlsx
@@ -173,7 +173,7 @@
     <t>Extension.extension</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
   <si>
     <t xml:space="preserve">Extension
@@ -1411,7 +1411,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s" s="2">
         <v>39</v>

</xml_diff>